<commit_message>
1 de 3 Array Mesas e Rodadas
</commit_message>
<xml_diff>
--- a/src/assets/logicaRodada.xlsx
+++ b/src/assets/logicaRodada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Documents\2022\FRONTEND\RodadaDeNegocios\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4336E605-CF19-4838-B458-18070B47BAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C18262-602B-4223-9ED9-6FB868712C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:AY74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5546875" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Logica aplicada em Rodada de Negocios
</commit_message>
<xml_diff>
--- a/src/assets/logicaRodada.xlsx
+++ b/src/assets/logicaRodada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Documents\2022\FRONTEND\RodadaDeNegocios\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C18262-602B-4223-9ED9-6FB868712C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D223B823-1C7B-4863-AED5-CAD7E48149F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1092" yWindow="5484" windowWidth="23040" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="173">
   <si>
     <t>1º Rodada</t>
   </si>
@@ -505,6 +505,57 @@
   </si>
   <si>
     <t>Mesa 10</t>
+  </si>
+  <si>
+    <t>[8,9,10,11,12,13,14]</t>
+  </si>
+  <si>
+    <t>[10,11,12,13,14,8,9]</t>
+  </si>
+  <si>
+    <t>[4,5,6,7,1,2,3]</t>
+  </si>
+  <si>
+    <t>[12,13,14,8,9,10,11]</t>
+  </si>
+  <si>
+    <t>RODADA 1</t>
+  </si>
+  <si>
+    <t>RODADA 2</t>
+  </si>
+  <si>
+    <t>RODADA 3</t>
+  </si>
+  <si>
+    <t>RODADA 4</t>
+  </si>
+  <si>
+    <t>[12,8,9,13,14,10,11]</t>
+  </si>
+  <si>
+    <t>[15,16,17,18,19,20,21]</t>
+  </si>
+  <si>
+    <t>[18,19,20,21,15,16,17]</t>
+  </si>
+  <si>
+    <t>[21,15,16,17,18,19,20]</t>
+  </si>
+  <si>
+    <t>[17,18,19,20,21,15,16]</t>
+  </si>
+  <si>
+    <t>[22,23,24,25,26,27,28]</t>
+  </si>
+  <si>
+    <t>[26,27,28,22,23,24,25]</t>
+  </si>
+  <si>
+    <t>[23,24,25,26,27,28,22]</t>
+  </si>
+  <si>
+    <t>[27,28,22,23,24,25,26]</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +2034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30F3509-C362-461C-A56D-D9FC10E267F0}">
   <dimension ref="A1:AY74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
@@ -5680,10 +5731,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Plan2"/>
-  <dimension ref="A1:AP58"/>
+  <dimension ref="A1:AM58"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8:AF8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5546875" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5694,9 +5745,11 @@
     <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
     <col min="28" max="28" width="9.5546875" customWidth="1"/>
+    <col min="36" max="38" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
@@ -5786,9 +5839,20 @@
       <c r="AI1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="AK1" s="25"/>
-    </row>
-    <row r="2" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5882,14 +5946,17 @@
       <c r="AJ2" t="s">
         <v>148</v>
       </c>
+      <c r="AK2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>152</v>
+      </c>
       <c r="AM2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -5980,14 +6047,20 @@
       <c r="AI3" s="15">
         <v>9</v>
       </c>
+      <c r="AJ3" t="s">
+        <v>156</v>
+      </c>
       <c r="AK3" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>159</v>
       </c>
       <c r="AM3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -6078,8 +6151,20 @@
       <c r="AI4" s="15">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -6170,8 +6255,20 @@
       <c r="AI5" s="15">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -6247,7 +6344,7 @@
       </c>
       <c r="AI6" s="16"/>
     </row>
-    <row r="7" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -6303,7 +6400,7 @@
       <c r="AH7" s="13"/>
       <c r="AI7" s="16"/>
     </row>
-    <row r="8" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -6361,7 +6458,7 @@
       <c r="AH8" s="13"/>
       <c r="AI8" s="16"/>
     </row>
-    <row r="9" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="J9" s="17"/>
       <c r="K9" s="13"/>
@@ -6390,7 +6487,7 @@
       <c r="AH9" s="13"/>
       <c r="AI9" s="16"/>
     </row>
-    <row r="10" spans="1:42" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:39" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A10" s="3"/>
       <c r="J10" s="17"/>
       <c r="K10" s="18" t="s">
@@ -6465,7 +6562,7 @@
         <v>+1</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -6565,7 +6662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -6665,7 +6762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -6765,7 +6862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -6865,7 +6962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -6941,7 +7038,7 @@
       <c r="AH15" s="12"/>
       <c r="AI15" s="15"/>
     </row>
-    <row r="16" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>

</xml_diff>